<commit_message>
no time to lose
</commit_message>
<xml_diff>
--- a/レポート/理論値.xlsx
+++ b/レポート/理論値.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nakayama/Dropbox (Personal)/授業2019/システム解析特論/レポート/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4CED0C-C92E-F149-91EF-11211B727F5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42BB563-C466-F744-B794-E7B201319FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{17A6EEAD-48DE-2246-BAE2-7D73442710A6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>平均到着率</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>システムA</t>
+  </si>
+  <si>
+    <t>システムB</t>
+  </si>
+  <si>
+    <t>システムC</t>
   </si>
 </sst>
 </file>
@@ -2632,10 +2641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2F7199-A647-6743-8C5A-831FFDA771D3}">
-  <dimension ref="C1:P13"/>
+  <dimension ref="C1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3016,6 +3025,65 @@
       </c>
       <c r="P13" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>0.17668600000000001</v>
+      </c>
+      <c r="F39">
+        <v>0.59756900000000002</v>
+      </c>
+      <c r="G39">
+        <v>0.2</v>
+      </c>
+      <c r="H39">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>0.507081</v>
+      </c>
+      <c r="F40">
+        <v>0.50390400000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41">
+        <v>0.19773499999999999</v>
+      </c>
+      <c r="F41">
+        <v>0.200348</v>
+      </c>
+      <c r="G41">
+        <v>0.2</v>
+      </c>
+      <c r="H41">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>